<commit_message>
Quang đẹp trai push code
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/Login.xlsx
+++ b/src/test/resources/datatest/Login.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QuangTester\MyProject\src\test\resources\datatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE379EF-EFE5-46BE-B1CE-EF58805A0D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D40A18-72CD-4ED0-97A1-A5E37F55B3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1522" yWindow="1522" windowWidth="19562" windowHeight="10161" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27183" yWindow="1100" windowWidth="19563" windowHeight="10162" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>EMAIL</t>
   </si>
@@ -365,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -393,9 +393,27 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{A43ECDB3-4CA9-4001-B73E-8581B5E34B54}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{8C17E622-1D9C-4DE9-965A-531A27446AF4}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{89A7FEA8-9E87-4238-BB30-3218AA6505E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>